<commit_message>
update demographics with new data for median ages for all data points, send old xlsx to archive, update internal review
</commit_message>
<xml_diff>
--- a/resources/ACS_PUMS/EDDT_Census2000PUMS.xlsx
+++ b/resources/ACS_PUMS/EDDT_Census2000PUMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nyco365-my.sharepoint.com/personal/emaurer_planning_nyc_gov/Documents/Attachments/EDDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{EC095141-A6F5-488C-B176-B78A7D541840}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8DC3A1-C1B5-435E-B22A-6A2801EFE655}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69D0806E-0C53-4FB4-A00E-29406900B0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74F5F581-8C02-41B6-B873-8E9B64C4BE29}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{74F5F581-8C02-41B6-B873-8E9B64C4BE29}"/>
   </bookViews>
   <sheets>
     <sheet name="Census00" sheetId="2" r:id="rId1"/>
@@ -1632,7 +1632,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1690,15 +1690,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2017,706 +2018,704 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F3910F-07A7-419B-A1B2-E3047D9A536F}">
   <dimension ref="A1:PJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="OA1" workbookViewId="0">
-      <selection activeCell="PH21" sqref="PH21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="10.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="10.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="64" max="65" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="69" max="70" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="79" max="80" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="89" max="90" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="94" max="95" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="99" max="100" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="104" max="105" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="109" max="110" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="99" max="100" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="109" max="110" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="114" max="115" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="10.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="114" max="115" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="119" max="120" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="119" max="120" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="124" max="125" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="10.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="129" max="130" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="129" max="130" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="132" max="133" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="134" max="135" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="139" max="140" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="144" max="145" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="149" max="150" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="132" max="133" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="134" max="135" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="139" max="140" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="144" max="145" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="149" max="150" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="153" max="153" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="154" max="155" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="159" max="160" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="164" max="165" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="169" max="170" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="154" max="155" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="159" max="160" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="10.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="164" max="165" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="169" max="170" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="172" max="172" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="174" max="175" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="174" max="175" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="176" max="176" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="179" max="180" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="184" max="185" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="189" max="190" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="194" max="195" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="184" max="185" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="189" max="190" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="194" max="195" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="198" max="198" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="199" max="200" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="199" max="200" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="204" max="205" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="209" max="210" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="214" max="215" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="219" max="220" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="209" max="210" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="214" max="215" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="219" max="220" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="223" max="223" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="224" max="225" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="224" max="225" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="227" max="227" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="229" max="230" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="229" max="230" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="231" max="231" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="234" max="235" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="239" max="240" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="244" max="245" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="249" max="250" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="251" max="252" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="254" max="255" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="259" max="260" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="234" max="235" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="9.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="239" max="240" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="244" max="245" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="249" max="250" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="251" max="252" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="254" max="255" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="259" max="260" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="263" max="263" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="264" max="265" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="264" max="265" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="267" max="267" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="269" max="270" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="10.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="269" max="270" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="271" max="271" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="272" max="272" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="274" max="275" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="274" max="275" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="276" max="276" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="279" max="280" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="283" max="283" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="284" max="285" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="284" max="285" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="287" max="287" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="288" max="288" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="289" max="290" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="292" max="292" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="294" max="295" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="289" max="290" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="292" max="292" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="294" max="295" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="296" max="296" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="297" max="297" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="298" max="298" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="299" max="300" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="301" max="301" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="299" max="300" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="301" max="301" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="303" max="303" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="304" max="305" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="309" max="310" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="311" max="311" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="314" max="315" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="316" max="316" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="319" max="320" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="304" max="305" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="8.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="309" max="310" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="311" max="311" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="312" max="312" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="313" max="313" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="314" max="315" width="9.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="316" max="316" width="9.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="317" max="317" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="319" max="320" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="321" max="321" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="323" max="323" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="324" max="325" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="326" max="326" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="328" max="328" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="329" max="330" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="331" max="331" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="332" max="332" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="324" max="325" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="326" max="326" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="327" max="327" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="328" max="328" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="329" max="330" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="331" max="331" width="7.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="332" max="332" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="333" max="333" width="7" style="10" bestFit="1" customWidth="1"/>
-    <col min="334" max="335" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="336" max="336" width="6.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="337" max="337" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="338" max="338" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="339" max="340" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="341" max="341" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="342" max="342" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="334" max="335" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="336" max="336" width="6.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="337" max="337" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="338" max="338" width="9.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="339" max="340" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="341" max="341" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="342" max="342" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="343" max="343" width="8.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="344" max="345" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="346" max="346" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="346" max="346" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="347" max="347" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="348" max="348" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="349" max="350" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="348" max="348" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="349" max="350" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="351" max="351" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="352" max="352" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="353" max="353" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="354" max="355" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="356" max="356" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="352" max="352" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="353" max="353" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="354" max="355" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="356" max="356" width="7.265625" style="10" bestFit="1" customWidth="1"/>
     <col min="357" max="357" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="358" max="358" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="359" max="360" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="358" max="358" width="8.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="359" max="360" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="361" max="361" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="362" max="362" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="363" max="363" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="364" max="365" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="366" max="366" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="367" max="367" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="368" max="368" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="369" max="370" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="371" max="371" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="372" max="372" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="362" max="362" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="363" max="363" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="364" max="365" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="366" max="366" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="367" max="367" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="368" max="368" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="369" max="370" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="371" max="371" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="372" max="372" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="373" max="373" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="374" max="375" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="376" max="376" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="377" max="377" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="378" max="378" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="379" max="380" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="381" max="381" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="382" max="382" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="383" max="383" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="384" max="385" width="5.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="386" max="386" width="5.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="387" max="387" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="388" max="388" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="389" max="390" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="391" max="391" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="392" max="392" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="393" max="393" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="394" max="395" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="396" max="396" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="397" max="397" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="398" max="398" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="399" max="400" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="401" max="401" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="402" max="402" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="403" max="403" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="404" max="405" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="406" max="406" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="407" max="407" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="408" max="408" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="409" max="410" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="411" max="411" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="412" max="412" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="413" max="413" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="414" max="415" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="416" max="416" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="417" max="417" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="418" max="418" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="419" max="420" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="421" max="421" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="422" max="422" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="423" max="423" width="7.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="424" max="425" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="426" max="426" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="374" max="375" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="376" max="376" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="377" max="377" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="378" max="378" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="379" max="380" width="6.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="381" max="381" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="382" max="382" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="383" max="383" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="384" max="385" width="5.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="386" max="386" width="5.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="387" max="387" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="388" max="388" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="389" max="390" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="391" max="391" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="392" max="392" width="7.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="393" max="393" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="394" max="395" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="396" max="396" width="7.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="397" max="397" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="398" max="398" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="399" max="400" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="401" max="401" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="402" max="402" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="403" max="403" width="7.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="404" max="405" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="406" max="406" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="407" max="407" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="408" max="408" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="409" max="410" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="411" max="411" width="7.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="412" max="412" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="413" max="413" width="7.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="414" max="415" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="416" max="416" width="6.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="417" max="417" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="418" max="418" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="419" max="420" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="421" max="421" width="7.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="422" max="422" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="423" max="423" width="7.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="424" max="425" width="6.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="426" max="426" width="6.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="427" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:426" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:426" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="27" t="s">
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="27" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="25" t="s">
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="27" t="s">
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="27" t="s">
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="27" t="s">
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="26"/>
-      <c r="AU1" s="27" t="s">
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AV1" s="25"/>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="26"/>
-      <c r="AZ1" s="27" t="s">
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="27"/>
+      <c r="AZ1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="BA1" s="25"/>
-      <c r="BB1" s="25"/>
-      <c r="BC1" s="25"/>
-      <c r="BD1" s="26"/>
-      <c r="BE1" s="27" t="s">
+      <c r="BA1" s="26"/>
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="26"/>
+      <c r="BD1" s="27"/>
+      <c r="BE1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="BF1" s="25"/>
-      <c r="BG1" s="25"/>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="27" t="s">
+      <c r="BF1" s="26"/>
+      <c r="BG1" s="26"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="27"/>
+      <c r="BJ1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="27" t="s">
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="27"/>
+      <c r="BO1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="27" t="s">
+      <c r="BP1" s="26"/>
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="27"/>
+      <c r="BT1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="27" t="s">
+      <c r="BU1" s="26"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="27"/>
+      <c r="BY1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
-      <c r="CB1" s="25"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="27" t="s">
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="27"/>
+      <c r="CD1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="CE1" s="25"/>
-      <c r="CF1" s="25"/>
-      <c r="CG1" s="25"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="27" t="s">
+      <c r="CE1" s="26"/>
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="27"/>
+      <c r="CI1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="CJ1" s="25"/>
-      <c r="CK1" s="25"/>
-      <c r="CL1" s="25"/>
-      <c r="CM1" s="26"/>
-      <c r="CN1" s="27" t="s">
+      <c r="CJ1" s="26"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="26"/>
+      <c r="CM1" s="27"/>
+      <c r="CN1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="CO1" s="25"/>
-      <c r="CP1" s="25"/>
-      <c r="CQ1" s="25"/>
-      <c r="CR1" s="26"/>
-      <c r="CS1" s="27" t="s">
+      <c r="CO1" s="26"/>
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="27"/>
+      <c r="CS1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="CT1" s="25"/>
-      <c r="CU1" s="25"/>
-      <c r="CV1" s="25"/>
-      <c r="CW1" s="26"/>
-      <c r="CX1" s="27" t="s">
+      <c r="CT1" s="26"/>
+      <c r="CU1" s="26"/>
+      <c r="CV1" s="26"/>
+      <c r="CW1" s="27"/>
+      <c r="CX1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="CY1" s="25"/>
-      <c r="CZ1" s="25"/>
-      <c r="DA1" s="25"/>
-      <c r="DB1" s="26"/>
-      <c r="DC1" s="27" t="s">
+      <c r="CY1" s="26"/>
+      <c r="CZ1" s="26"/>
+      <c r="DA1" s="26"/>
+      <c r="DB1" s="27"/>
+      <c r="DC1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="DD1" s="25"/>
-      <c r="DE1" s="25"/>
-      <c r="DF1" s="25"/>
-      <c r="DG1" s="26"/>
-      <c r="DH1" s="27" t="s">
+      <c r="DD1" s="26"/>
+      <c r="DE1" s="26"/>
+      <c r="DF1" s="26"/>
+      <c r="DG1" s="27"/>
+      <c r="DH1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="DI1" s="25"/>
-      <c r="DJ1" s="25"/>
-      <c r="DK1" s="25"/>
-      <c r="DL1" s="26"/>
-      <c r="DM1" s="27" t="s">
+      <c r="DI1" s="26"/>
+      <c r="DJ1" s="26"/>
+      <c r="DK1" s="26"/>
+      <c r="DL1" s="27"/>
+      <c r="DM1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="DN1" s="25"/>
-      <c r="DO1" s="25"/>
-      <c r="DP1" s="25"/>
-      <c r="DQ1" s="26"/>
-      <c r="DR1" s="27" t="s">
+      <c r="DN1" s="26"/>
+      <c r="DO1" s="26"/>
+      <c r="DP1" s="26"/>
+      <c r="DQ1" s="27"/>
+      <c r="DR1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="DS1" s="25"/>
-      <c r="DT1" s="25"/>
-      <c r="DU1" s="25"/>
-      <c r="DV1" s="25"/>
-      <c r="DW1" s="25" t="s">
+      <c r="DS1" s="26"/>
+      <c r="DT1" s="26"/>
+      <c r="DU1" s="26"/>
+      <c r="DV1" s="26"/>
+      <c r="DW1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="DX1" s="25"/>
-      <c r="DY1" s="25"/>
-      <c r="DZ1" s="25"/>
-      <c r="EA1" s="26"/>
-      <c r="EB1" s="27" t="s">
+      <c r="DX1" s="26"/>
+      <c r="DY1" s="26"/>
+      <c r="DZ1" s="26"/>
+      <c r="EA1" s="27"/>
+      <c r="EB1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="EC1" s="25"/>
-      <c r="ED1" s="25"/>
-      <c r="EE1" s="25"/>
-      <c r="EF1" s="26"/>
-      <c r="EG1" s="27" t="s">
+      <c r="EC1" s="26"/>
+      <c r="ED1" s="26"/>
+      <c r="EE1" s="26"/>
+      <c r="EF1" s="27"/>
+      <c r="EG1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="EH1" s="25"/>
-      <c r="EI1" s="25"/>
-      <c r="EJ1" s="25"/>
-      <c r="EK1" s="26"/>
-      <c r="EL1" s="27" t="s">
+      <c r="EH1" s="26"/>
+      <c r="EI1" s="26"/>
+      <c r="EJ1" s="26"/>
+      <c r="EK1" s="27"/>
+      <c r="EL1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="EM1" s="25"/>
-      <c r="EN1" s="25"/>
-      <c r="EO1" s="25"/>
-      <c r="EP1" s="26"/>
-      <c r="EQ1" s="27" t="s">
+      <c r="EM1" s="26"/>
+      <c r="EN1" s="26"/>
+      <c r="EO1" s="26"/>
+      <c r="EP1" s="27"/>
+      <c r="EQ1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="ER1" s="25"/>
-      <c r="ES1" s="25"/>
-      <c r="ET1" s="25"/>
-      <c r="EU1" s="26"/>
-      <c r="EV1" s="27" t="s">
+      <c r="ER1" s="26"/>
+      <c r="ES1" s="26"/>
+      <c r="ET1" s="26"/>
+      <c r="EU1" s="27"/>
+      <c r="EV1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="EW1" s="25"/>
-      <c r="EX1" s="25"/>
-      <c r="EY1" s="25"/>
-      <c r="EZ1" s="26"/>
-      <c r="FA1" s="27" t="s">
+      <c r="EW1" s="26"/>
+      <c r="EX1" s="26"/>
+      <c r="EY1" s="26"/>
+      <c r="EZ1" s="27"/>
+      <c r="FA1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="FB1" s="25"/>
-      <c r="FC1" s="25"/>
-      <c r="FD1" s="25"/>
-      <c r="FE1" s="26"/>
-      <c r="FF1" s="27" t="s">
+      <c r="FB1" s="26"/>
+      <c r="FC1" s="26"/>
+      <c r="FD1" s="26"/>
+      <c r="FE1" s="27"/>
+      <c r="FF1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="FG1" s="25"/>
-      <c r="FH1" s="25"/>
-      <c r="FI1" s="25"/>
-      <c r="FJ1" s="26"/>
-      <c r="FK1" s="27" t="s">
+      <c r="FG1" s="26"/>
+      <c r="FH1" s="26"/>
+      <c r="FI1" s="26"/>
+      <c r="FJ1" s="27"/>
+      <c r="FK1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="FL1" s="25"/>
-      <c r="FM1" s="25"/>
-      <c r="FN1" s="25"/>
-      <c r="FO1" s="26"/>
-      <c r="FP1" s="27" t="s">
+      <c r="FL1" s="26"/>
+      <c r="FM1" s="26"/>
+      <c r="FN1" s="26"/>
+      <c r="FO1" s="27"/>
+      <c r="FP1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="FQ1" s="25"/>
-      <c r="FR1" s="25"/>
-      <c r="FS1" s="25"/>
-      <c r="FT1" s="26"/>
-      <c r="FU1" s="27" t="s">
+      <c r="FQ1" s="26"/>
+      <c r="FR1" s="26"/>
+      <c r="FS1" s="26"/>
+      <c r="FT1" s="27"/>
+      <c r="FU1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="FV1" s="25"/>
-      <c r="FW1" s="25"/>
-      <c r="FX1" s="25"/>
-      <c r="FY1" s="26"/>
-      <c r="FZ1" s="27" t="s">
+      <c r="FV1" s="26"/>
+      <c r="FW1" s="26"/>
+      <c r="FX1" s="26"/>
+      <c r="FY1" s="27"/>
+      <c r="FZ1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="GA1" s="25"/>
-      <c r="GB1" s="25"/>
-      <c r="GC1" s="25"/>
-      <c r="GD1" s="26"/>
-      <c r="GE1" s="27" t="s">
+      <c r="GA1" s="26"/>
+      <c r="GB1" s="26"/>
+      <c r="GC1" s="26"/>
+      <c r="GD1" s="27"/>
+      <c r="GE1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="GF1" s="25"/>
-      <c r="GG1" s="25"/>
-      <c r="GH1" s="25"/>
-      <c r="GI1" s="26"/>
-      <c r="GJ1" s="27" t="s">
+      <c r="GF1" s="26"/>
+      <c r="GG1" s="26"/>
+      <c r="GH1" s="26"/>
+      <c r="GI1" s="27"/>
+      <c r="GJ1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="GK1" s="25"/>
-      <c r="GL1" s="25"/>
-      <c r="GM1" s="25"/>
-      <c r="GN1" s="26"/>
-      <c r="GO1" s="27" t="s">
+      <c r="GK1" s="26"/>
+      <c r="GL1" s="26"/>
+      <c r="GM1" s="26"/>
+      <c r="GN1" s="27"/>
+      <c r="GO1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="GP1" s="25"/>
-      <c r="GQ1" s="25"/>
-      <c r="GR1" s="25"/>
-      <c r="GS1" s="26"/>
-      <c r="GT1" s="27" t="s">
+      <c r="GP1" s="26"/>
+      <c r="GQ1" s="26"/>
+      <c r="GR1" s="26"/>
+      <c r="GS1" s="27"/>
+      <c r="GT1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="GU1" s="25"/>
-      <c r="GV1" s="25"/>
-      <c r="GW1" s="25"/>
-      <c r="GX1" s="26"/>
-      <c r="GY1" s="27" t="s">
+      <c r="GU1" s="26"/>
+      <c r="GV1" s="26"/>
+      <c r="GW1" s="26"/>
+      <c r="GX1" s="27"/>
+      <c r="GY1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="GZ1" s="25"/>
-      <c r="HA1" s="25"/>
-      <c r="HB1" s="25"/>
-      <c r="HC1" s="26"/>
-      <c r="HD1" s="27" t="s">
+      <c r="GZ1" s="26"/>
+      <c r="HA1" s="26"/>
+      <c r="HB1" s="26"/>
+      <c r="HC1" s="27"/>
+      <c r="HD1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="HE1" s="25"/>
-      <c r="HF1" s="25"/>
-      <c r="HG1" s="25"/>
-      <c r="HH1" s="26"/>
-      <c r="HI1" s="27" t="s">
+      <c r="HE1" s="26"/>
+      <c r="HF1" s="26"/>
+      <c r="HG1" s="26"/>
+      <c r="HH1" s="27"/>
+      <c r="HI1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="HJ1" s="25"/>
-      <c r="HK1" s="25"/>
-      <c r="HL1" s="25"/>
-      <c r="HM1" s="26"/>
-      <c r="HN1" s="27" t="s">
+      <c r="HJ1" s="26"/>
+      <c r="HK1" s="26"/>
+      <c r="HL1" s="26"/>
+      <c r="HM1" s="27"/>
+      <c r="HN1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="HO1" s="25"/>
-      <c r="HP1" s="25"/>
-      <c r="HQ1" s="25"/>
-      <c r="HR1" s="26"/>
-      <c r="HS1" s="27" t="s">
+      <c r="HO1" s="26"/>
+      <c r="HP1" s="26"/>
+      <c r="HQ1" s="26"/>
+      <c r="HR1" s="27"/>
+      <c r="HS1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="HT1" s="25"/>
-      <c r="HU1" s="25"/>
-      <c r="HV1" s="25"/>
-      <c r="HW1" s="26"/>
-      <c r="HX1" s="27" t="s">
+      <c r="HT1" s="26"/>
+      <c r="HU1" s="26"/>
+      <c r="HV1" s="26"/>
+      <c r="HW1" s="27"/>
+      <c r="HX1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="HY1" s="25"/>
-      <c r="HZ1" s="25"/>
-      <c r="IA1" s="25"/>
-      <c r="IB1" s="26"/>
-      <c r="IC1" s="27" t="s">
+      <c r="HY1" s="26"/>
+      <c r="HZ1" s="26"/>
+      <c r="IA1" s="26"/>
+      <c r="IB1" s="27"/>
+      <c r="IC1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="ID1" s="25"/>
-      <c r="IE1" s="25"/>
-      <c r="IF1" s="25"/>
-      <c r="IG1" s="26"/>
-      <c r="IH1" s="27" t="s">
+      <c r="ID1" s="26"/>
+      <c r="IE1" s="26"/>
+      <c r="IF1" s="26"/>
+      <c r="IG1" s="27"/>
+      <c r="IH1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="II1" s="25"/>
-      <c r="IJ1" s="25"/>
-      <c r="IK1" s="25"/>
-      <c r="IL1" s="26"/>
-      <c r="IM1" s="27" t="s">
+      <c r="II1" s="26"/>
+      <c r="IJ1" s="26"/>
+      <c r="IK1" s="26"/>
+      <c r="IL1" s="27"/>
+      <c r="IM1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="IN1" s="25"/>
-      <c r="IO1" s="25"/>
-      <c r="IP1" s="25"/>
-      <c r="IQ1" s="26"/>
+      <c r="IN1" s="26"/>
+      <c r="IO1" s="26"/>
+      <c r="IP1" s="26"/>
+      <c r="IQ1" s="27"/>
       <c r="IR1" s="22" t="s">
         <v>50</v>
       </c>
@@ -2963,7 +2962,7 @@
       <c r="PI1" s="23"/>
       <c r="PJ1" s="24"/>
     </row>
-    <row r="2" spans="1:426" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:426" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="3" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>451</v>
       </c>
@@ -4308,13 +4307,13 @@
         <v>0.1</v>
       </c>
       <c r="V3" s="9">
-        <v>42.9</v>
-      </c>
-      <c r="W3" s="15">
-        <v>0</v>
-      </c>
-      <c r="X3" s="15">
-        <v>0</v>
+        <v>34.5</v>
+      </c>
+      <c r="W3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="X3" s="28">
+        <v>0.2</v>
       </c>
       <c r="Y3" s="16"/>
       <c r="Z3" s="14"/>
@@ -5503,7 +5502,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>453</v>
       </c>
@@ -5568,13 +5567,13 @@
         <v>0.2</v>
       </c>
       <c r="V4" s="9">
-        <v>33.5</v>
-      </c>
-      <c r="W4" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="X4" s="15">
-        <v>0.2</v>
+        <v>31.4</v>
+      </c>
+      <c r="W4" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="X4" s="28">
+        <v>0.6</v>
       </c>
       <c r="Y4" s="16"/>
       <c r="Z4" s="14"/>
@@ -6763,7 +6762,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>454</v>
       </c>
@@ -6828,13 +6827,13 @@
         <v>0.2</v>
       </c>
       <c r="V5" s="9">
-        <v>42.6</v>
-      </c>
-      <c r="W5" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="X5" s="15">
-        <v>0.1</v>
+        <v>33.5</v>
+      </c>
+      <c r="W5" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="X5" s="28">
+        <v>0.4</v>
       </c>
       <c r="Y5" s="16"/>
       <c r="Z5" s="14"/>
@@ -8023,7 +8022,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>455</v>
       </c>
@@ -8088,13 +8087,13 @@
         <v>0.2</v>
       </c>
       <c r="V6" s="9">
-        <v>47.2</v>
-      </c>
-      <c r="W6" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="X6" s="15">
-        <v>0.1</v>
+        <v>35.9</v>
+      </c>
+      <c r="W6" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="X6" s="28">
+        <v>0.3</v>
       </c>
       <c r="Y6" s="16"/>
       <c r="Z6" s="14"/>
@@ -9283,7 +9282,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>456</v>
       </c>
@@ -9348,13 +9347,13 @@
         <v>0.2</v>
       </c>
       <c r="V7" s="9">
-        <v>43.1</v>
-      </c>
-      <c r="W7" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="X7" s="15">
-        <v>0.1</v>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="W7" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="X7" s="28">
+        <v>0.3</v>
       </c>
       <c r="Y7" s="16"/>
       <c r="Z7" s="14"/>
@@ -10543,7 +10542,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>457</v>
       </c>
@@ -10608,13 +10607,13 @@
         <v>0.4</v>
       </c>
       <c r="V8" s="9">
-        <v>63.8</v>
-      </c>
-      <c r="W8" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="X8" s="15">
-        <v>0.1</v>
+        <v>36.1</v>
+      </c>
+      <c r="W8" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="X8" s="28">
+        <v>0.7</v>
       </c>
       <c r="Y8" s="16"/>
       <c r="Z8" s="14"/>
@@ -11803,7 +11802,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>3701</v>
       </c>
@@ -11868,13 +11867,13 @@
         <v>1</v>
       </c>
       <c r="V9" s="9">
-        <v>48.9</v>
-      </c>
-      <c r="W9" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X9" s="15">
-        <v>0.4</v>
+        <v>37.1</v>
+      </c>
+      <c r="W9" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X9" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y9" s="16"/>
       <c r="Z9" s="14"/>
@@ -13063,7 +13062,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="10" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>3702</v>
       </c>
@@ -13128,13 +13127,13 @@
         <v>0.8</v>
       </c>
       <c r="V10" s="9">
-        <v>34</v>
-      </c>
-      <c r="W10" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X10" s="15">
-        <v>0.4</v>
+        <v>33.4</v>
+      </c>
+      <c r="W10" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X10" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y10" s="16"/>
       <c r="Z10" s="14"/>
@@ -14323,7 +14322,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>3703</v>
       </c>
@@ -14388,13 +14387,13 @@
         <v>1</v>
       </c>
       <c r="V11" s="9">
-        <v>55.1</v>
-      </c>
-      <c r="W11" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X11" s="15">
-        <v>0.3</v>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="W11" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X11" s="28">
+        <v>1.4</v>
       </c>
       <c r="Y11" s="16"/>
       <c r="Z11" s="14"/>
@@ -15583,7 +15582,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>3704</v>
       </c>
@@ -15648,13 +15647,13 @@
         <v>0.9</v>
       </c>
       <c r="V12" s="9">
-        <v>45.2</v>
-      </c>
-      <c r="W12" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X12" s="15">
-        <v>0.3</v>
+        <v>36</v>
+      </c>
+      <c r="W12" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X12" s="28">
+        <v>1.4</v>
       </c>
       <c r="Y12" s="16"/>
       <c r="Z12" s="14"/>
@@ -16843,7 +16842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>3705</v>
       </c>
@@ -16908,13 +16907,13 @@
         <v>0.6</v>
       </c>
       <c r="V13" s="9">
-        <v>26.3</v>
-      </c>
-      <c r="W13" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X13" s="15">
-        <v>0.5</v>
+        <v>26.4</v>
+      </c>
+      <c r="W13" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X13" s="28">
+        <v>1.8</v>
       </c>
       <c r="Y13" s="16"/>
       <c r="Z13" s="14"/>
@@ -18103,7 +18102,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>3706</v>
       </c>
@@ -18168,13 +18167,13 @@
         <v>0.7</v>
       </c>
       <c r="V14" s="9">
-        <v>29.5</v>
-      </c>
-      <c r="W14" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X14" s="15">
-        <v>0.4</v>
+        <v>28.9</v>
+      </c>
+      <c r="W14" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X14" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y14" s="16"/>
       <c r="Z14" s="14"/>
@@ -19363,7 +19362,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>3707</v>
       </c>
@@ -19428,13 +19427,13 @@
         <v>0.5</v>
       </c>
       <c r="V15" s="9">
-        <v>25.9</v>
-      </c>
-      <c r="W15" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X15" s="15">
-        <v>0.5</v>
+        <v>27.1</v>
+      </c>
+      <c r="W15" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X15" s="28">
+        <v>1.8</v>
       </c>
       <c r="Y15" s="16"/>
       <c r="Z15" s="14"/>
@@ -20623,7 +20622,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>3708</v>
       </c>
@@ -20688,13 +20687,13 @@
         <v>0.7</v>
       </c>
       <c r="V16" s="9">
-        <v>27.5</v>
-      </c>
-      <c r="W16" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X16" s="15">
-        <v>0.4</v>
+        <v>29.1</v>
+      </c>
+      <c r="W16" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X16" s="28">
+        <v>1.9</v>
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="14"/>
@@ -21883,7 +21882,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>3709</v>
       </c>
@@ -21948,13 +21947,13 @@
         <v>0.6</v>
       </c>
       <c r="V17" s="9">
-        <v>30.7</v>
-      </c>
-      <c r="W17" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X17" s="15">
-        <v>0.4</v>
+        <v>31.8</v>
+      </c>
+      <c r="W17" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X17" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y17" s="16"/>
       <c r="Z17" s="14"/>
@@ -23143,7 +23142,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>3710</v>
       </c>
@@ -23208,13 +23207,13 @@
         <v>0.6</v>
       </c>
       <c r="V18" s="9">
-        <v>26.8</v>
-      </c>
-      <c r="W18" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X18" s="15">
-        <v>0.5</v>
+        <v>28.3</v>
+      </c>
+      <c r="W18" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X18" s="28">
+        <v>1.7</v>
       </c>
       <c r="Y18" s="16"/>
       <c r="Z18" s="14"/>
@@ -24403,7 +24402,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="19" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>3801</v>
       </c>
@@ -24468,13 +24467,13 @@
         <v>0.6</v>
       </c>
       <c r="V19" s="9">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="W19" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X19" s="15">
-        <v>0.4</v>
+        <v>33</v>
+      </c>
+      <c r="W19" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X19" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y19" s="16"/>
       <c r="Z19" s="14"/>
@@ -25663,7 +25662,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>3802</v>
       </c>
@@ -25728,13 +25727,13 @@
         <v>0.8</v>
       </c>
       <c r="V20" s="9">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="W20" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X20" s="15">
-        <v>0.5</v>
+        <v>31.2</v>
+      </c>
+      <c r="W20" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X20" s="28">
+        <v>1.6</v>
       </c>
       <c r="Y20" s="16"/>
       <c r="Z20" s="14"/>
@@ -26923,7 +26922,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>3803</v>
       </c>
@@ -26988,13 +26987,13 @@
         <v>0.9</v>
       </c>
       <c r="V21" s="9">
-        <v>31.5</v>
-      </c>
-      <c r="W21" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X21" s="15">
-        <v>0.4</v>
+        <v>33.9</v>
+      </c>
+      <c r="W21" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X21" s="28">
+        <v>1.4</v>
       </c>
       <c r="Y21" s="16"/>
       <c r="Z21" s="14"/>
@@ -28183,7 +28182,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="22" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>3804</v>
       </c>
@@ -28248,13 +28247,13 @@
         <v>0.8</v>
       </c>
       <c r="V22" s="9">
-        <v>32.1</v>
-      </c>
-      <c r="W22" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X22" s="15">
-        <v>0.4</v>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W22" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X22" s="28">
+        <v>1.7</v>
       </c>
       <c r="Y22" s="16"/>
       <c r="Z22" s="14"/>
@@ -29443,7 +29442,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>3805</v>
       </c>
@@ -29508,13 +29507,13 @@
         <v>0.7</v>
       </c>
       <c r="V23" s="9">
-        <v>71</v>
-      </c>
-      <c r="W23" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X23" s="15">
-        <v>0.3</v>
+        <v>38.4</v>
+      </c>
+      <c r="W23" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X23" s="28">
+        <v>0.8</v>
       </c>
       <c r="Y23" s="16"/>
       <c r="Z23" s="14"/>
@@ -30703,7 +30702,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="24" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>3806</v>
       </c>
@@ -30768,13 +30767,13 @@
         <v>0.7</v>
       </c>
       <c r="V24" s="9">
-        <v>61.6</v>
-      </c>
-      <c r="W24" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X24" s="15">
-        <v>0.3</v>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="W24" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X24" s="28">
+        <v>0.8</v>
       </c>
       <c r="Y24" s="16"/>
       <c r="Z24" s="14"/>
@@ -31963,7 +31962,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="25" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>3807</v>
       </c>
@@ -32028,13 +32027,13 @@
         <v>0.8</v>
       </c>
       <c r="V25" s="9">
-        <v>53.5</v>
-      </c>
-      <c r="W25" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="X25" s="15">
-        <v>0.5</v>
+        <v>37</v>
+      </c>
+      <c r="W25" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X25" s="28">
+        <v>1</v>
       </c>
       <c r="Y25" s="16"/>
       <c r="Z25" s="14"/>
@@ -33223,7 +33222,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="26" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>3808</v>
       </c>
@@ -33288,13 +33287,13 @@
         <v>0.8</v>
       </c>
       <c r="V26" s="9">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="W26" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="X26" s="15">
-        <v>0.5</v>
+        <v>39</v>
+      </c>
+      <c r="W26" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X26" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y26" s="16"/>
       <c r="Z26" s="14"/>
@@ -34483,7 +34482,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="27" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>3809</v>
       </c>
@@ -34548,13 +34547,13 @@
         <v>0.8</v>
       </c>
       <c r="V27" s="9">
-        <v>40.4</v>
-      </c>
-      <c r="W27" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X27" s="15">
-        <v>0.5</v>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="W27" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X27" s="28">
+        <v>1</v>
       </c>
       <c r="Y27" s="16"/>
       <c r="Z27" s="14"/>
@@ -35743,7 +35742,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="28" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>3810</v>
       </c>
@@ -35808,13 +35807,13 @@
         <v>0.8</v>
       </c>
       <c r="V28" s="9">
-        <v>60.6</v>
-      </c>
-      <c r="W28" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="X28" s="15">
-        <v>0.5</v>
+        <v>35.6</v>
+      </c>
+      <c r="W28" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X28" s="28">
+        <v>1</v>
       </c>
       <c r="Y28" s="16"/>
       <c r="Z28" s="14"/>
@@ -37003,7 +37002,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="29" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>3901</v>
       </c>
@@ -37068,13 +37067,13 @@
         <v>0.7</v>
       </c>
       <c r="V29" s="9">
-        <v>74.8</v>
-      </c>
-      <c r="W29" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X29" s="15">
-        <v>0.2</v>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="W29" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X29" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y29" s="16"/>
       <c r="Z29" s="14"/>
@@ -38263,7 +38262,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="30" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>3902</v>
       </c>
@@ -38328,13 +38327,13 @@
         <v>0.8</v>
       </c>
       <c r="V30" s="9">
-        <v>68</v>
-      </c>
-      <c r="W30" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X30" s="15">
-        <v>0.3</v>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="W30" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X30" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y30" s="16"/>
       <c r="Z30" s="14"/>
@@ -39523,7 +39522,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="31" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>3903</v>
       </c>
@@ -39588,13 +39587,13 @@
         <v>0.7</v>
       </c>
       <c r="V31" s="9">
-        <v>49.1</v>
-      </c>
-      <c r="W31" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X31" s="15">
-        <v>0.2</v>
+        <v>34.200000000000003</v>
+      </c>
+      <c r="W31" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X31" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y31" s="16"/>
       <c r="Z31" s="14"/>
@@ -40783,7 +40782,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>4001</v>
       </c>
@@ -40848,13 +40847,13 @@
         <v>0.7</v>
       </c>
       <c r="V32" s="9">
-        <v>46.9</v>
-      </c>
-      <c r="W32" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X32" s="15">
-        <v>0.3</v>
+        <v>30.7</v>
+      </c>
+      <c r="W32" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X32" s="28">
+        <v>1.4</v>
       </c>
       <c r="Y32" s="16"/>
       <c r="Z32" s="14"/>
@@ -42043,7 +42042,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="33" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>4002</v>
       </c>
@@ -42108,13 +42107,13 @@
         <v>0.7</v>
       </c>
       <c r="V33" s="9">
-        <v>26.2</v>
-      </c>
-      <c r="W33" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X33" s="15">
-        <v>0.5</v>
+        <v>27.5</v>
+      </c>
+      <c r="W33" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X33" s="28">
+        <v>1.8</v>
       </c>
       <c r="Y33" s="16"/>
       <c r="Z33" s="14"/>
@@ -43303,7 +43302,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>4003</v>
       </c>
@@ -43368,13 +43367,13 @@
         <v>0.7</v>
       </c>
       <c r="V34" s="9">
-        <v>29</v>
-      </c>
-      <c r="W34" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X34" s="15">
-        <v>0.4</v>
+        <v>29.9</v>
+      </c>
+      <c r="W34" s="28">
+        <v>1</v>
+      </c>
+      <c r="X34" s="28">
+        <v>2</v>
       </c>
       <c r="Y34" s="16"/>
       <c r="Z34" s="14"/>
@@ -44563,7 +44562,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="35" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>4004</v>
       </c>
@@ -44628,13 +44627,13 @@
         <v>0.8</v>
       </c>
       <c r="V35" s="9">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="W35" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X35" s="15">
-        <v>0.5</v>
+        <v>33.5</v>
+      </c>
+      <c r="W35" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X35" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y35" s="16"/>
       <c r="Z35" s="14"/>
@@ -45823,7 +45822,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="36" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>4005</v>
       </c>
@@ -45888,13 +45887,13 @@
         <v>0.8</v>
       </c>
       <c r="V36" s="9">
-        <v>47.3</v>
-      </c>
-      <c r="W36" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X36" s="15">
-        <v>0.4</v>
+        <v>34.4</v>
+      </c>
+      <c r="W36" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X36" s="28">
+        <v>0.9</v>
       </c>
       <c r="Y36" s="16"/>
       <c r="Z36" s="14"/>
@@ -47083,7 +47082,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="37" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>4006</v>
       </c>
@@ -47148,13 +47147,13 @@
         <v>0.8</v>
       </c>
       <c r="V37" s="9">
-        <v>31.6</v>
-      </c>
-      <c r="W37" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X37" s="15">
-        <v>0.4</v>
+        <v>31.9</v>
+      </c>
+      <c r="W37" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X37" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y37" s="16"/>
       <c r="Z37" s="14"/>
@@ -48343,7 +48342,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>4007</v>
       </c>
@@ -48408,13 +48407,13 @@
         <v>0.7</v>
       </c>
       <c r="V38" s="9">
-        <v>26.2</v>
-      </c>
-      <c r="W38" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X38" s="15">
-        <v>0.5</v>
+        <v>27.1</v>
+      </c>
+      <c r="W38" s="28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X38" s="28">
+        <v>2.5</v>
       </c>
       <c r="Y38" s="16"/>
       <c r="Z38" s="14"/>
@@ -49603,7 +49602,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="39" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>4008</v>
       </c>
@@ -49668,13 +49667,13 @@
         <v>0.7</v>
       </c>
       <c r="V39" s="9">
-        <v>30.2</v>
-      </c>
-      <c r="W39" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X39" s="15">
-        <v>0.4</v>
+        <v>29.9</v>
+      </c>
+      <c r="W39" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X39" s="28">
+        <v>1.8</v>
       </c>
       <c r="Y39" s="16"/>
       <c r="Z39" s="14"/>
@@ -50863,7 +50862,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="40" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>4009</v>
       </c>
@@ -50928,13 +50927,13 @@
         <v>0.6</v>
       </c>
       <c r="V40" s="9">
-        <v>43.5</v>
-      </c>
-      <c r="W40" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X40" s="15">
-        <v>0.3</v>
+        <v>35.4</v>
+      </c>
+      <c r="W40" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X40" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y40" s="16"/>
       <c r="Z40" s="14"/>
@@ -52123,7 +52122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
         <v>4010</v>
       </c>
@@ -52188,13 +52187,13 @@
         <v>0.7</v>
       </c>
       <c r="V41" s="9">
-        <v>30.9</v>
-      </c>
-      <c r="W41" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X41" s="15">
-        <v>0.4</v>
+        <v>33.1</v>
+      </c>
+      <c r="W41" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X41" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y41" s="16"/>
       <c r="Z41" s="14"/>
@@ -53383,7 +53382,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="42" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>4011</v>
       </c>
@@ -53450,11 +53449,11 @@
       <c r="V42" s="9">
         <v>33.700000000000003</v>
       </c>
-      <c r="W42" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X42" s="15">
-        <v>0.4</v>
+      <c r="W42" s="28">
+        <v>1</v>
+      </c>
+      <c r="X42" s="28">
+        <v>1.8</v>
       </c>
       <c r="Y42" s="16"/>
       <c r="Z42" s="14"/>
@@ -54643,7 +54642,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="43" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>4012</v>
       </c>
@@ -54708,13 +54707,13 @@
         <v>0.7</v>
       </c>
       <c r="V43" s="9">
-        <v>36.4</v>
-      </c>
-      <c r="W43" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X43" s="15">
-        <v>0.3</v>
+        <v>32</v>
+      </c>
+      <c r="W43" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X43" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y43" s="16"/>
       <c r="Z43" s="14"/>
@@ -55903,7 +55902,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="44" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>4013</v>
       </c>
@@ -55968,13 +55967,13 @@
         <v>0.9</v>
       </c>
       <c r="V44" s="9">
-        <v>67.3</v>
-      </c>
-      <c r="W44" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X44" s="15">
-        <v>0.3</v>
+        <v>38.4</v>
+      </c>
+      <c r="W44" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X44" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y44" s="16"/>
       <c r="Z44" s="14"/>
@@ -57163,7 +57162,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="45" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>4014</v>
       </c>
@@ -57228,13 +57227,13 @@
         <v>0.8</v>
       </c>
       <c r="V45" s="9">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="W45" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X45" s="15">
-        <v>0.2</v>
+        <v>29.6</v>
+      </c>
+      <c r="W45" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X45" s="28">
+        <v>1.6</v>
       </c>
       <c r="Y45" s="16"/>
       <c r="Z45" s="14"/>
@@ -58423,7 +58422,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>4015</v>
       </c>
@@ -58488,13 +58487,13 @@
         <v>0.7</v>
       </c>
       <c r="V46" s="9">
-        <v>43</v>
-      </c>
-      <c r="W46" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X46" s="15">
-        <v>0.3</v>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="W46" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X46" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y46" s="16"/>
       <c r="Z46" s="14"/>
@@ -59683,7 +59682,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="47" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>4016</v>
       </c>
@@ -59748,13 +59747,13 @@
         <v>0.9</v>
       </c>
       <c r="V47" s="9">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="W47" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X47" s="15">
-        <v>0.2</v>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="W47" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X47" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y47" s="16"/>
       <c r="Z47" s="14"/>
@@ -60943,7 +60942,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="48" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>4017</v>
       </c>
@@ -61008,13 +61007,13 @@
         <v>0.8</v>
       </c>
       <c r="V48" s="9">
-        <v>65.3</v>
-      </c>
-      <c r="W48" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X48" s="15">
-        <v>0.2</v>
+        <v>38.799999999999997</v>
+      </c>
+      <c r="W48" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X48" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y48" s="16"/>
       <c r="Z48" s="14"/>
@@ -62203,7 +62202,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="49" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>4018</v>
       </c>
@@ -62268,13 +62267,13 @@
         <v>1</v>
       </c>
       <c r="V49" s="9">
-        <v>64.3</v>
-      </c>
-      <c r="W49" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X49" s="15">
-        <v>0.2</v>
+        <v>39.9</v>
+      </c>
+      <c r="W49" s="28">
+        <v>1</v>
+      </c>
+      <c r="X49" s="28">
+        <v>1.5</v>
       </c>
       <c r="Y49" s="16"/>
       <c r="Z49" s="14"/>
@@ -63463,7 +63462,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="50" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>4101</v>
       </c>
@@ -63528,13 +63527,13 @@
         <v>0.7</v>
       </c>
       <c r="V50" s="9">
-        <v>46</v>
-      </c>
-      <c r="W50" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X50" s="15">
-        <v>0.3</v>
+        <v>34.1</v>
+      </c>
+      <c r="W50" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X50" s="28">
+        <v>0.9</v>
       </c>
       <c r="Y50" s="16"/>
       <c r="Z50" s="14"/>
@@ -64723,7 +64722,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="51" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>4102</v>
       </c>
@@ -64788,13 +64787,13 @@
         <v>0.7</v>
       </c>
       <c r="V51" s="9">
-        <v>34.1</v>
-      </c>
-      <c r="W51" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X51" s="15">
-        <v>0.4</v>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="W51" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X51" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y51" s="16"/>
       <c r="Z51" s="14"/>
@@ -65983,7 +65982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>4103</v>
       </c>
@@ -66048,13 +66047,13 @@
         <v>0.7</v>
       </c>
       <c r="V52" s="9">
-        <v>49.3</v>
-      </c>
-      <c r="W52" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X52" s="15">
-        <v>0.2</v>
+        <v>39</v>
+      </c>
+      <c r="W52" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X52" s="28">
+        <v>0.8</v>
       </c>
       <c r="Y52" s="16"/>
       <c r="Z52" s="14"/>
@@ -67243,7 +67242,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="53" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>4104</v>
       </c>
@@ -67308,13 +67307,13 @@
         <v>1</v>
       </c>
       <c r="V53" s="9">
-        <v>62</v>
-      </c>
-      <c r="W53" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X53" s="15">
-        <v>0.3</v>
+        <v>41.3</v>
+      </c>
+      <c r="W53" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X53" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y53" s="16"/>
       <c r="Z53" s="14"/>
@@ -68503,7 +68502,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="54" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>4105</v>
       </c>
@@ -68568,13 +68567,13 @@
         <v>0.7</v>
       </c>
       <c r="V54" s="9">
-        <v>39</v>
-      </c>
-      <c r="W54" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X54" s="15">
-        <v>0.3</v>
+        <v>36.6</v>
+      </c>
+      <c r="W54" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X54" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y54" s="16"/>
       <c r="Z54" s="14"/>
@@ -69763,7 +69762,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>4106</v>
       </c>
@@ -69828,13 +69827,13 @@
         <v>0.8</v>
       </c>
       <c r="V55" s="9">
-        <v>46.8</v>
-      </c>
-      <c r="W55" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X55" s="15">
-        <v>0.3</v>
+        <v>37.1</v>
+      </c>
+      <c r="W55" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X55" s="28">
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y55" s="16"/>
       <c r="Z55" s="14"/>
@@ -71023,7 +71022,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="56" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>4107</v>
       </c>
@@ -71088,13 +71087,13 @@
         <v>0.7</v>
       </c>
       <c r="V56" s="9">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="W56" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X56" s="15">
-        <v>0.4</v>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="W56" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X56" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y56" s="16"/>
       <c r="Z56" s="14"/>
@@ -72283,7 +72282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>4108</v>
       </c>
@@ -72348,13 +72347,13 @@
         <v>1</v>
       </c>
       <c r="V57" s="9">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="W57" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="X57" s="15">
-        <v>0.4</v>
+        <v>41</v>
+      </c>
+      <c r="W57" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="X57" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y57" s="16"/>
       <c r="Z57" s="14"/>
@@ -73543,7 +73542,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="58" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>4109</v>
       </c>
@@ -73608,13 +73607,13 @@
         <v>0.8</v>
       </c>
       <c r="V58" s="9">
-        <v>39</v>
-      </c>
-      <c r="W58" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X58" s="15">
-        <v>0.3</v>
+        <v>35.1</v>
+      </c>
+      <c r="W58" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="X58" s="28">
+        <v>1</v>
       </c>
       <c r="Y58" s="16"/>
       <c r="Z58" s="14"/>
@@ -74803,7 +74802,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="59" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
         <v>4110</v>
       </c>
@@ -74868,13 +74867,13 @@
         <v>0.7</v>
       </c>
       <c r="V59" s="9">
-        <v>60.6</v>
-      </c>
-      <c r="W59" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X59" s="15">
-        <v>0.2</v>
+        <v>36</v>
+      </c>
+      <c r="W59" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X59" s="28">
+        <v>1.2</v>
       </c>
       <c r="Y59" s="16"/>
       <c r="Z59" s="14"/>
@@ -76063,7 +76062,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="60" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
         <v>4111</v>
       </c>
@@ -76128,13 +76127,13 @@
         <v>0.7</v>
       </c>
       <c r="V60" s="9">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="W60" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X60" s="15">
-        <v>0.3</v>
+        <v>33.4</v>
+      </c>
+      <c r="W60" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X60" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y60" s="16"/>
       <c r="Z60" s="14"/>
@@ -77323,7 +77322,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A61" s="11">
         <v>4112</v>
       </c>
@@ -77388,13 +77387,13 @@
         <v>0.6</v>
       </c>
       <c r="V61" s="9">
-        <v>31.7</v>
-      </c>
-      <c r="W61" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="X61" s="15">
-        <v>0.4</v>
+        <v>33.9</v>
+      </c>
+      <c r="W61" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="X61" s="28">
+        <v>1.3</v>
       </c>
       <c r="Y61" s="16"/>
       <c r="Z61" s="14"/>
@@ -78583,7 +78582,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="62" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>4113</v>
       </c>
@@ -78648,13 +78647,13 @@
         <v>0.8</v>
       </c>
       <c r="V62" s="9">
-        <v>43.3</v>
-      </c>
-      <c r="W62" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X62" s="15">
-        <v>0.4</v>
+        <v>34.9</v>
+      </c>
+      <c r="W62" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="X62" s="28">
+        <v>1.4</v>
       </c>
       <c r="Y62" s="16"/>
       <c r="Z62" s="14"/>
@@ -79843,7 +79842,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:426" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:426" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>4114</v>
       </c>
@@ -79908,13 +79907,13 @@
         <v>1</v>
       </c>
       <c r="V63" s="9">
-        <v>46.9</v>
-      </c>
-      <c r="W63" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="X63" s="15">
-        <v>0.4</v>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="W63" s="28">
+        <v>1</v>
+      </c>
+      <c r="X63" s="28">
+        <v>1.7</v>
       </c>
       <c r="Y63" s="16"/>
       <c r="Z63" s="14"/>
@@ -81105,69 +81104,12 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="MX1:NB1"/>
-    <mergeCell ref="NC1:NG1"/>
-    <mergeCell ref="NH1:NL1"/>
-    <mergeCell ref="LT1:LX1"/>
-    <mergeCell ref="LY1:MC1"/>
-    <mergeCell ref="MD1:MH1"/>
-    <mergeCell ref="MI1:MM1"/>
-    <mergeCell ref="MN1:MR1"/>
-    <mergeCell ref="MS1:MW1"/>
-    <mergeCell ref="LO1:LS1"/>
-    <mergeCell ref="JL1:JP1"/>
-    <mergeCell ref="JQ1:JU1"/>
-    <mergeCell ref="JV1:JZ1"/>
-    <mergeCell ref="KA1:KE1"/>
-    <mergeCell ref="KF1:KJ1"/>
-    <mergeCell ref="KK1:KO1"/>
-    <mergeCell ref="KP1:KT1"/>
-    <mergeCell ref="KU1:KY1"/>
-    <mergeCell ref="KZ1:LD1"/>
-    <mergeCell ref="LE1:LI1"/>
-    <mergeCell ref="LJ1:LN1"/>
-    <mergeCell ref="JG1:JK1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="HN1:HR1"/>
-    <mergeCell ref="HS1:HW1"/>
-    <mergeCell ref="HX1:IB1"/>
-    <mergeCell ref="IC1:IG1"/>
-    <mergeCell ref="IH1:IL1"/>
-    <mergeCell ref="IM1:IQ1"/>
-    <mergeCell ref="IR1:IV1"/>
-    <mergeCell ref="IW1:JA1"/>
-    <mergeCell ref="JB1:JF1"/>
-    <mergeCell ref="GY1:HC1"/>
-    <mergeCell ref="EV1:EZ1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FF1:FJ1"/>
-    <mergeCell ref="FK1:FO1"/>
-    <mergeCell ref="FP1:FT1"/>
-    <mergeCell ref="FU1:FY1"/>
-    <mergeCell ref="FZ1:GD1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GJ1:GN1"/>
-    <mergeCell ref="GO1:GS1"/>
-    <mergeCell ref="GT1:GX1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="EQ1:EU1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="DR1:DV1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EB1:EF1"/>
-    <mergeCell ref="EG1:EK1"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="PF1:PJ1"/>
+    <mergeCell ref="OG1:OK1"/>
+    <mergeCell ref="OL1:OP1"/>
+    <mergeCell ref="OQ1:OU1"/>
+    <mergeCell ref="OV1:OZ1"/>
+    <mergeCell ref="PA1:PE1"/>
     <mergeCell ref="AA1:AE1"/>
     <mergeCell ref="NM1:NQ1"/>
     <mergeCell ref="NR1:NV1"/>
@@ -81184,18 +81126,84 @@
     <mergeCell ref="BO1:BS1"/>
     <mergeCell ref="BT1:BX1"/>
     <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="PF1:PJ1"/>
-    <mergeCell ref="OG1:OK1"/>
-    <mergeCell ref="OL1:OP1"/>
-    <mergeCell ref="OQ1:OU1"/>
-    <mergeCell ref="OV1:OZ1"/>
-    <mergeCell ref="PA1:PE1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="EQ1:EU1"/>
+    <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DH1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="DR1:DV1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EB1:EF1"/>
+    <mergeCell ref="EG1:EK1"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="GY1:HC1"/>
+    <mergeCell ref="EV1:EZ1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FF1:FJ1"/>
+    <mergeCell ref="FK1:FO1"/>
+    <mergeCell ref="FP1:FT1"/>
+    <mergeCell ref="FU1:FY1"/>
+    <mergeCell ref="FZ1:GD1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="GJ1:GN1"/>
+    <mergeCell ref="GO1:GS1"/>
+    <mergeCell ref="GT1:GX1"/>
+    <mergeCell ref="JG1:JK1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="HN1:HR1"/>
+    <mergeCell ref="HS1:HW1"/>
+    <mergeCell ref="HX1:IB1"/>
+    <mergeCell ref="IC1:IG1"/>
+    <mergeCell ref="IH1:IL1"/>
+    <mergeCell ref="IM1:IQ1"/>
+    <mergeCell ref="IR1:IV1"/>
+    <mergeCell ref="IW1:JA1"/>
+    <mergeCell ref="JB1:JF1"/>
+    <mergeCell ref="LO1:LS1"/>
+    <mergeCell ref="JL1:JP1"/>
+    <mergeCell ref="JQ1:JU1"/>
+    <mergeCell ref="JV1:JZ1"/>
+    <mergeCell ref="KA1:KE1"/>
+    <mergeCell ref="KF1:KJ1"/>
+    <mergeCell ref="KK1:KO1"/>
+    <mergeCell ref="KP1:KT1"/>
+    <mergeCell ref="KU1:KY1"/>
+    <mergeCell ref="KZ1:LD1"/>
+    <mergeCell ref="LE1:LI1"/>
+    <mergeCell ref="LJ1:LN1"/>
+    <mergeCell ref="MX1:NB1"/>
+    <mergeCell ref="NC1:NG1"/>
+    <mergeCell ref="NH1:NL1"/>
+    <mergeCell ref="LT1:LX1"/>
+    <mergeCell ref="LY1:MC1"/>
+    <mergeCell ref="MD1:MH1"/>
+    <mergeCell ref="MI1:MM1"/>
+    <mergeCell ref="MN1:MR1"/>
+    <mergeCell ref="MS1:MW1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AC4EC9EEC787747A21020991D7C5A0C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9591f2c22eb77891f7786dab03d70d3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a006254a-362b-4ff4-965e-371f488d1924" xmlns:ns4="0974b3c8-8b09-43c3-8cba-9a7da3221e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7207b9d247d4a80ce5df938cda55a91" ns3:_="" ns4:_="">
     <xsd:import namespace="a006254a-362b-4ff4-965e-371f488d1924"/>
@@ -81404,15 +81412,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -81420,6 +81419,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E8A1F6-7505-4204-B639-F74A5958FB26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC9E0B5-FFE9-496A-9382-155D202B9A1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -81438,27 +81445,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E8A1F6-7505-4204-B639-F74A5958FB26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D826C3B8-8DAB-4048-9691-AEF6D8514417}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0974b3c8-8b09-43c3-8cba-9a7da3221e79"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="a006254a-362b-4ff4-965e-371f488d1924"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0974b3c8-8b09-43c3-8cba-9a7da3221e79"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>